<commit_message>
Added regions to district lookup files
</commit_message>
<xml_diff>
--- a/district_lookup/uganda_districts_2020.xlsx
+++ b/district_lookup/uganda_districts_2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hman\Repo\uvotedata\Cleaned\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hman\Repo\kalulu21\district_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48098F2E-BF7A-4E5A-A3E1-043B2273A4DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A630CDF-CBAD-465B-95D2-63C29C6DBD48}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49E75B13-90DF-4644-BDF0-439DEF152917}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="154">
   <si>
     <t>district_code</t>
   </si>
@@ -469,6 +469,24 @@
   </si>
   <si>
     <t>ZOMBO</t>
+  </si>
+  <si>
+    <t>region_code</t>
+  </si>
+  <si>
+    <t>region_name</t>
+  </si>
+  <si>
+    <t>NORTHERN</t>
+  </si>
+  <si>
+    <t>EASTERN</t>
+  </si>
+  <si>
+    <t>WESTERN</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
   </si>
 </sst>
 </file>
@@ -820,1192 +838,2076 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA57DBE-E820-4341-BA15-E66CF9ED3726}">
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>88</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>123</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>109</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>98</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>89</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>117</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>99</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>118</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>90</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>139</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>91</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>137</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>6</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>145</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>61</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>62</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>138</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>63</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>54</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>113</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>114</v>
       </c>
       <c r="B50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>129</v>
       </c>
       <c r="B51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>11</v>
       </c>
       <c r="B52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>64</v>
       </c>
       <c r="B53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>100</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>12</v>
       </c>
       <c r="B55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>13</v>
       </c>
       <c r="B56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>46</v>
       </c>
       <c r="B57" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>14</v>
       </c>
       <c r="B59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>124</v>
       </c>
       <c r="B60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>130</v>
       </c>
       <c r="B61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>125</v>
       </c>
       <c r="B63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>43</v>
       </c>
       <c r="B64" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>47</v>
       </c>
       <c r="B65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>131</v>
       </c>
       <c r="B66" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>16</v>
       </c>
       <c r="B67" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>17</v>
       </c>
       <c r="B68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>102</v>
       </c>
       <c r="B69" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>126</v>
       </c>
       <c r="B70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>92</v>
       </c>
       <c r="B72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>18</v>
       </c>
       <c r="B73" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>132</v>
       </c>
       <c r="B74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>19</v>
       </c>
       <c r="B75" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>66</v>
       </c>
       <c r="B76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>103</v>
       </c>
       <c r="B77" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>20</v>
       </c>
       <c r="B78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>21</v>
       </c>
       <c r="B79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>127</v>
       </c>
       <c r="B80" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>104</v>
       </c>
       <c r="B81" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>93</v>
       </c>
       <c r="B82" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>84</v>
       </c>
       <c r="B83" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>48</v>
       </c>
       <c r="B84" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>119</v>
       </c>
       <c r="B85" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>22</v>
       </c>
       <c r="B87" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>144</v>
       </c>
       <c r="B88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>94</v>
       </c>
       <c r="B89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>23</v>
       </c>
       <c r="B90" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>105</v>
       </c>
       <c r="B91" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>80</v>
       </c>
       <c r="B92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>133</v>
       </c>
       <c r="B93" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>67</v>
       </c>
       <c r="B94" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>77</v>
       </c>
       <c r="B95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>24</v>
       </c>
       <c r="B96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>141</v>
       </c>
       <c r="B97" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>25</v>
       </c>
       <c r="B98" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>49</v>
       </c>
       <c r="B99" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>26</v>
       </c>
       <c r="B100" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>142</v>
       </c>
       <c r="B101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>27</v>
       </c>
       <c r="B102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>140</v>
       </c>
       <c r="B103" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>106</v>
       </c>
       <c r="B104" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>68</v>
       </c>
       <c r="B105" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>28</v>
       </c>
       <c r="B106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>29</v>
       </c>
       <c r="B107" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>30</v>
       </c>
       <c r="B108" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>31</v>
       </c>
       <c r="B109" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>32</v>
       </c>
       <c r="B110" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>128</v>
       </c>
       <c r="B111" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111">
+        <v>3</v>
+      </c>
+      <c r="D111" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>56</v>
       </c>
       <c r="B112" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <v>3</v>
+      </c>
+      <c r="D112" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>69</v>
       </c>
       <c r="B113" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>44</v>
       </c>
       <c r="B114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>95</v>
       </c>
       <c r="B115" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>120</v>
       </c>
       <c r="B116" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>75</v>
       </c>
       <c r="B117" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>107</v>
       </c>
       <c r="B118" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>33</v>
       </c>
       <c r="B119" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <v>3</v>
+      </c>
+      <c r="D119" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>108</v>
       </c>
       <c r="B120" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>96</v>
       </c>
       <c r="B121" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <v>4</v>
+      </c>
+      <c r="D121" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>34</v>
       </c>
       <c r="B122" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <v>4</v>
+      </c>
+      <c r="D122" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>110</v>
       </c>
       <c r="B123" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <v>3</v>
+      </c>
+      <c r="D123" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>134</v>
       </c>
       <c r="B124" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>115</v>
       </c>
       <c r="B125" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>86</v>
       </c>
       <c r="B126" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>76</v>
       </c>
       <c r="B127" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <v>3</v>
+      </c>
+      <c r="D127" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>50</v>
       </c>
       <c r="B128" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <v>3</v>
+      </c>
+      <c r="D128" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>121</v>
       </c>
       <c r="B129" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <v>3</v>
+      </c>
+      <c r="D129" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>35</v>
       </c>
       <c r="B130" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>36</v>
       </c>
       <c r="B131" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>116</v>
       </c>
       <c r="B132" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <v>4</v>
+      </c>
+      <c r="D132" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>112</v>
       </c>
       <c r="B133" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <v>4</v>
+      </c>
+      <c r="D133" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>122</v>
       </c>
       <c r="B134" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <v>4</v>
+      </c>
+      <c r="D134" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>37</v>
       </c>
       <c r="B135" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <v>4</v>
+      </c>
+      <c r="D135" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <v>4</v>
+      </c>
+      <c r="D136" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>97</v>
       </c>
       <c r="B137" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>101</v>
       </c>
       <c r="B138" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <v>4</v>
+      </c>
+      <c r="D138" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>51</v>
       </c>
       <c r="B139" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>38</v>
       </c>
       <c r="B140" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>146</v>
       </c>
       <c r="B141" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>45</v>
       </c>
       <c r="B142" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>143</v>
       </c>
       <c r="B143" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>39</v>
       </c>
       <c r="B144" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>52</v>
       </c>
       <c r="B145" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>53</v>
       </c>
       <c r="B146" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C146">
+        <v>3</v>
+      </c>
+      <c r="D146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>87</v>
       </c>
       <c r="B147" t="s">
         <v>147</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+      <c r="D147" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to District Lookup Files, Resending 2016 district & Subcounty files (#3)
Updates to District Lookup Files, Resending 2016 district & Subcounty files while adding regions to district files
</commit_message>
<xml_diff>
--- a/district_lookup/uganda_districts_2020.xlsx
+++ b/district_lookup/uganda_districts_2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hman\Repo\uvotedata\Cleaned\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hman\Repo\kalulu21\district_lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48098F2E-BF7A-4E5A-A3E1-043B2273A4DF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A630CDF-CBAD-465B-95D2-63C29C6DBD48}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49E75B13-90DF-4644-BDF0-439DEF152917}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="154">
   <si>
     <t>district_code</t>
   </si>
@@ -469,6 +469,24 @@
   </si>
   <si>
     <t>ZOMBO</t>
+  </si>
+  <si>
+    <t>region_code</t>
+  </si>
+  <si>
+    <t>region_name</t>
+  </si>
+  <si>
+    <t>NORTHERN</t>
+  </si>
+  <si>
+    <t>EASTERN</t>
+  </si>
+  <si>
+    <t>WESTERN</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
   </si>
 </sst>
 </file>
@@ -820,1192 +838,2076 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA57DBE-E820-4341-BA15-E66CF9ED3726}">
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>70</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>111</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>88</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>57</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>81</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>58</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>71</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>78</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>41</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>123</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>109</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>82</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>79</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>98</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>89</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>73</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>117</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>60</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>99</v>
       </c>
       <c r="B29" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>118</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>90</v>
       </c>
       <c r="B31" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>139</v>
       </c>
       <c r="B34" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>91</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>5</v>
       </c>
       <c r="B36" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>137</v>
       </c>
       <c r="B37" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>6</v>
       </c>
       <c r="B38" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>145</v>
       </c>
       <c r="B39" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>61</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>7</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>62</v>
       </c>
       <c r="B42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>138</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>63</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>54</v>
       </c>
       <c r="B48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>113</v>
       </c>
       <c r="B49" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>114</v>
       </c>
       <c r="B50" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>129</v>
       </c>
       <c r="B51" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>11</v>
       </c>
       <c r="B52" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>64</v>
       </c>
       <c r="B53" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>100</v>
       </c>
       <c r="B54" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>12</v>
       </c>
       <c r="B55" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>13</v>
       </c>
       <c r="B56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>46</v>
       </c>
       <c r="B57" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>55</v>
       </c>
       <c r="B58" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>14</v>
       </c>
       <c r="B59" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>124</v>
       </c>
       <c r="B60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>130</v>
       </c>
       <c r="B61" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>3</v>
+      </c>
+      <c r="D61" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>125</v>
       </c>
       <c r="B63" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>43</v>
       </c>
       <c r="B64" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>47</v>
       </c>
       <c r="B65" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>131</v>
       </c>
       <c r="B66" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>16</v>
       </c>
       <c r="B67" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>17</v>
       </c>
       <c r="B68" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>102</v>
       </c>
       <c r="B69" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>126</v>
       </c>
       <c r="B70" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>92</v>
       </c>
       <c r="B72" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>18</v>
       </c>
       <c r="B73" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>132</v>
       </c>
       <c r="B74" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>19</v>
       </c>
       <c r="B75" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>66</v>
       </c>
       <c r="B76" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>103</v>
       </c>
       <c r="B77" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>20</v>
       </c>
       <c r="B78" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>21</v>
       </c>
       <c r="B79" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>127</v>
       </c>
       <c r="B80" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>104</v>
       </c>
       <c r="B81" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>93</v>
       </c>
       <c r="B82" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>84</v>
       </c>
       <c r="B83" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>48</v>
       </c>
       <c r="B84" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>119</v>
       </c>
       <c r="B85" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>1</v>
+      </c>
+      <c r="D85" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>22</v>
       </c>
       <c r="B87" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>144</v>
       </c>
       <c r="B88" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>94</v>
       </c>
       <c r="B89" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>23</v>
       </c>
       <c r="B90" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>105</v>
       </c>
       <c r="B91" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>80</v>
       </c>
       <c r="B92" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>133</v>
       </c>
       <c r="B93" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C93">
+        <v>3</v>
+      </c>
+      <c r="D93" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>67</v>
       </c>
       <c r="B94" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C94">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>77</v>
       </c>
       <c r="B95" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>24</v>
       </c>
       <c r="B96" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>141</v>
       </c>
       <c r="B97" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>25</v>
       </c>
       <c r="B98" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C98">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>49</v>
       </c>
       <c r="B99" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C99">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>26</v>
       </c>
       <c r="B100" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C100">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>142</v>
       </c>
       <c r="B101" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C101">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>27</v>
       </c>
       <c r="B102" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C102">
+        <v>4</v>
+      </c>
+      <c r="D102" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>140</v>
       </c>
       <c r="B103" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C103">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>106</v>
       </c>
       <c r="B104" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C104">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>68</v>
       </c>
       <c r="B105" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>28</v>
       </c>
       <c r="B106" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C106">
+        <v>3</v>
+      </c>
+      <c r="D106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>29</v>
       </c>
       <c r="B107" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C107">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>30</v>
       </c>
       <c r="B108" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>31</v>
       </c>
       <c r="B109" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>32</v>
       </c>
       <c r="B110" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>128</v>
       </c>
       <c r="B111" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C111">
+        <v>3</v>
+      </c>
+      <c r="D111" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>56</v>
       </c>
       <c r="B112" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C112">
+        <v>3</v>
+      </c>
+      <c r="D112" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>69</v>
       </c>
       <c r="B113" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>44</v>
       </c>
       <c r="B114" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>95</v>
       </c>
       <c r="B115" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C115">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>120</v>
       </c>
       <c r="B116" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C116">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>75</v>
       </c>
       <c r="B117" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C117">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>107</v>
       </c>
       <c r="B118" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C118">
+        <v>3</v>
+      </c>
+      <c r="D118" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>33</v>
       </c>
       <c r="B119" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C119">
+        <v>3</v>
+      </c>
+      <c r="D119" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>108</v>
       </c>
       <c r="B120" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C120">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>96</v>
       </c>
       <c r="B121" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C121">
+        <v>4</v>
+      </c>
+      <c r="D121" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>34</v>
       </c>
       <c r="B122" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C122">
+        <v>4</v>
+      </c>
+      <c r="D122" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>110</v>
       </c>
       <c r="B123" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C123">
+        <v>3</v>
+      </c>
+      <c r="D123" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>134</v>
       </c>
       <c r="B124" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C124">
+        <v>3</v>
+      </c>
+      <c r="D124" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>115</v>
       </c>
       <c r="B125" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C125">
+        <v>3</v>
+      </c>
+      <c r="D125" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>86</v>
       </c>
       <c r="B126" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C126">
+        <v>3</v>
+      </c>
+      <c r="D126" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>76</v>
       </c>
       <c r="B127" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C127">
+        <v>3</v>
+      </c>
+      <c r="D127" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>50</v>
       </c>
       <c r="B128" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C128">
+        <v>3</v>
+      </c>
+      <c r="D128" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>121</v>
       </c>
       <c r="B129" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C129">
+        <v>3</v>
+      </c>
+      <c r="D129" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>35</v>
       </c>
       <c r="B130" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C130">
+        <v>2</v>
+      </c>
+      <c r="D130" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>36</v>
       </c>
       <c r="B131" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>116</v>
       </c>
       <c r="B132" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C132">
+        <v>4</v>
+      </c>
+      <c r="D132" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>112</v>
       </c>
       <c r="B133" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C133">
+        <v>4</v>
+      </c>
+      <c r="D133" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>122</v>
       </c>
       <c r="B134" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C134">
+        <v>4</v>
+      </c>
+      <c r="D134" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>37</v>
       </c>
       <c r="B135" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C135">
+        <v>4</v>
+      </c>
+      <c r="D135" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C136">
+        <v>4</v>
+      </c>
+      <c r="D136" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>97</v>
       </c>
       <c r="B137" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C137">
+        <v>2</v>
+      </c>
+      <c r="D137" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>101</v>
       </c>
       <c r="B138" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C138">
+        <v>4</v>
+      </c>
+      <c r="D138" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>51</v>
       </c>
       <c r="B139" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C139">
+        <v>2</v>
+      </c>
+      <c r="D139" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>38</v>
       </c>
       <c r="B140" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C140">
+        <v>2</v>
+      </c>
+      <c r="D140" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>146</v>
       </c>
       <c r="B141" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>45</v>
       </c>
       <c r="B142" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>143</v>
       </c>
       <c r="B143" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>39</v>
       </c>
       <c r="B144" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C144">
+        <v>2</v>
+      </c>
+      <c r="D144" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>52</v>
       </c>
       <c r="B145" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="D145" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>53</v>
       </c>
       <c r="B146" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C146">
+        <v>3</v>
+      </c>
+      <c r="D146" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>87</v>
       </c>
       <c r="B147" t="s">
         <v>147</v>
+      </c>
+      <c r="C147">
+        <v>3</v>
+      </c>
+      <c r="D147" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>